<commit_message>
General Improvements and Bug Fixes
- Suppressed errors from popping up in the terminal
- updated 'help' command to display hal capabilities
- disable_tts has been fixed
- added 'quit' option for 'analyze' function
- added 'graphing' functionality
- added graph of figure 2 training data.
- training data has been updated
- matplotlib library has been added for graphing
- graphing logic added in math.py
- removed playsound and replaced it with pygame library
- README.txt has been updated.
- requirements.txt now showcase all required libraries
- security policy has been updated. only supporting v1.1.6 and after.
- setup.py has been updated. Script checks if user has the libraries before attempting to install them. Also, the user can now choose if they want to install all the libraries at once or do the standard route.
</commit_message>
<xml_diff>
--- a/logic/SpaCy/training_data.xlsx
+++ b/logic/SpaCy/training_data.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henry\Desktop\chatbot-1.1.3\logic\SpaCy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0287816D-5493-4CA6-B656-8CB9DABCCB60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246FF5F2-725A-4533-A691-A784613AB4AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6000" yWindow="2115" windowWidth="16410" windowHeight="11295" xr2:uid="{94CEDFB2-1B98-48F3-8218-CEFE20B1FBF4}"/>
+    <workbookView xWindow="28695" yWindow="6330" windowWidth="16410" windowHeight="14145" xr2:uid="{94CEDFB2-1B98-48F3-8218-CEFE20B1FBF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="876">
   <si>
     <t>cls</t>
   </si>
@@ -1741,6 +1740,930 @@
   </si>
   <si>
     <t>I want you to repeat what I say</t>
+  </si>
+  <si>
+    <t>so tell me who are you</t>
+  </si>
+  <si>
+    <t>so who are you exactly</t>
+  </si>
+  <si>
+    <t>who exactly are you</t>
+  </si>
+  <si>
+    <t>what the hell is your name</t>
+  </si>
+  <si>
+    <t>what do you call yourself</t>
+  </si>
+  <si>
+    <t>can you clear the screen its getting a little cluttered</t>
+  </si>
+  <si>
+    <t>choose a random number for me</t>
+  </si>
+  <si>
+    <t>calculate compount interest for me</t>
+  </si>
+  <si>
+    <t>give me a random number</t>
+  </si>
+  <si>
+    <t>whats my name dude</t>
+  </si>
+  <si>
+    <t>convert hours to weeks to days to hours to minutes</t>
+  </si>
+  <si>
+    <t>I need to compute compount interest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remind me to </t>
+  </si>
+  <si>
+    <t>select a number at random</t>
+  </si>
+  <si>
+    <t>generate lottery numbers for me</t>
+  </si>
+  <si>
+    <t>hello there</t>
+  </si>
+  <si>
+    <t>can you remind me of my name</t>
+  </si>
+  <si>
+    <t>calculate hours in weeks</t>
+  </si>
+  <si>
+    <t>can you help me with compound interest</t>
+  </si>
+  <si>
+    <t>set a reminder for</t>
+  </si>
+  <si>
+    <t>pick a number at random</t>
+  </si>
+  <si>
+    <t>give me some lottery numbers</t>
+  </si>
+  <si>
+    <t>lets play rock paper scissors</t>
+  </si>
+  <si>
+    <t>good morning</t>
+  </si>
+  <si>
+    <t>could you tell me what my name is</t>
+  </si>
+  <si>
+    <t>im feeling fantastic today</t>
+  </si>
+  <si>
+    <t>calculate hours in days</t>
+  </si>
+  <si>
+    <t>can you help me with compound interest calculations</t>
+  </si>
+  <si>
+    <t>I needto be reminded to</t>
+  </si>
+  <si>
+    <t>search on wikipedia please</t>
+  </si>
+  <si>
+    <t>pick a number randomly</t>
+  </si>
+  <si>
+    <t>I need lottery numbers</t>
+  </si>
+  <si>
+    <t>roll a dice for me</t>
+  </si>
+  <si>
+    <t>I challenge you to a game of rock paper scissors</t>
+  </si>
+  <si>
+    <t>hi</t>
+  </si>
+  <si>
+    <t>do you know my name by chance</t>
+  </si>
+  <si>
+    <t>im in a great mood</t>
+  </si>
+  <si>
+    <t>calculate hours to</t>
+  </si>
+  <si>
+    <t>determine the compound interest on my savings</t>
+  </si>
+  <si>
+    <t>can you remind me to</t>
+  </si>
+  <si>
+    <t>look up something on wikipedia</t>
+  </si>
+  <si>
+    <t>generate a random number</t>
+  </si>
+  <si>
+    <t>can you generate some lottery numbers</t>
+  </si>
+  <si>
+    <t>give me a dice roll</t>
+  </si>
+  <si>
+    <t>rock paper scissors shoot</t>
+  </si>
+  <si>
+    <t>hey whats up</t>
+  </si>
+  <si>
+    <t>what do you have on file as my name</t>
+  </si>
+  <si>
+    <t>I apologize for that</t>
+  </si>
+  <si>
+    <t>im feeling awesome</t>
+  </si>
+  <si>
+    <t>go to youtube</t>
+  </si>
+  <si>
+    <t>open the GPT website</t>
+  </si>
+  <si>
+    <t>determine the equivalent of hours in weeks days hours minutes</t>
+  </si>
+  <si>
+    <t>how much will my investment grow with compound interest</t>
+  </si>
+  <si>
+    <t>remember to remind me about</t>
+  </si>
+  <si>
+    <t>find information about on wikipedia</t>
+  </si>
+  <si>
+    <t>I need a random number</t>
+  </si>
+  <si>
+    <t>pick lottery numbers for me</t>
+  </si>
+  <si>
+    <t>roll the dice please</t>
+  </si>
+  <si>
+    <t>wanna play rock paper scissors</t>
+  </si>
+  <si>
+    <t>hi there dude</t>
+  </si>
+  <si>
+    <t>whats your fucking name</t>
+  </si>
+  <si>
+    <t>I forgot my name can you tell me</t>
+  </si>
+  <si>
+    <t>im sorry for that</t>
+  </si>
+  <si>
+    <t>todays a great day</t>
+  </si>
+  <si>
+    <t>okay so whats your current hobby</t>
+  </si>
+  <si>
+    <t>access youtube</t>
+  </si>
+  <si>
+    <t>open the chat gpt website</t>
+  </si>
+  <si>
+    <t>find out how many weeks days hors and minutes are in a certain number of hours</t>
+  </si>
+  <si>
+    <t>compute the compound interest rate for me</t>
+  </si>
+  <si>
+    <t>I want a reminder for</t>
+  </si>
+  <si>
+    <t>get details on a topic from wikipedia</t>
+  </si>
+  <si>
+    <t>could you choose a number randomly</t>
+  </si>
+  <si>
+    <t>generate random lottery numbers</t>
+  </si>
+  <si>
+    <t>I need to roll a dice</t>
+  </si>
+  <si>
+    <t>create a picture for me</t>
+  </si>
+  <si>
+    <t>rock beats scissors paper covers rock lets play</t>
+  </si>
+  <si>
+    <t>yo</t>
+  </si>
+  <si>
+    <t>may I ask your name</t>
+  </si>
+  <si>
+    <t>what name do you have for me</t>
+  </si>
+  <si>
+    <t>sorry about that</t>
+  </si>
+  <si>
+    <t>im feeling on top of the world</t>
+  </si>
+  <si>
+    <t>alright what is your hobby</t>
+  </si>
+  <si>
+    <t>load youtube</t>
+  </si>
+  <si>
+    <t>take me to the chat gpt website</t>
+  </si>
+  <si>
+    <t>can you say what im saying</t>
+  </si>
+  <si>
+    <t>get the breakdown of hours into weeks days hours and minutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">find out the compound interest </t>
+  </si>
+  <si>
+    <t>don’t let me forget to</t>
+  </si>
+  <si>
+    <t>wikipedia topic</t>
+  </si>
+  <si>
+    <t>random number please</t>
+  </si>
+  <si>
+    <t>choose lottery numbers for me</t>
+  </si>
+  <si>
+    <t>can you roll a dice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generate a picture </t>
+  </si>
+  <si>
+    <t>tell me a joke please</t>
+  </si>
+  <si>
+    <t>how about a game of rock paper scissors</t>
+  </si>
+  <si>
+    <t>good afternoon</t>
+  </si>
+  <si>
+    <t>can you tell me your name</t>
+  </si>
+  <si>
+    <t>what did I input as my name</t>
+  </si>
+  <si>
+    <t>my apologies for that</t>
+  </si>
+  <si>
+    <t>am good</t>
+  </si>
+  <si>
+    <t>so whats your hobbies</t>
+  </si>
+  <si>
+    <t>take me to youtube</t>
+  </si>
+  <si>
+    <t>launch the chat gpt website</t>
+  </si>
+  <si>
+    <t>echo my words</t>
+  </si>
+  <si>
+    <t>convert hours to weeks days hours and minutes</t>
+  </si>
+  <si>
+    <t>I want to know how compound interest works</t>
+  </si>
+  <si>
+    <t>put a reminder on my calendar for</t>
+  </si>
+  <si>
+    <t>can you find the wikipedia page for a topic</t>
+  </si>
+  <si>
+    <t>select a number randomly for me</t>
+  </si>
+  <si>
+    <t>I want to play the lottery give me some numbers</t>
+  </si>
+  <si>
+    <t>roll a six-sides dice</t>
+  </si>
+  <si>
+    <t>I need an image</t>
+  </si>
+  <si>
+    <t>I could use a laugh tell me a joke</t>
+  </si>
+  <si>
+    <t>rock paper or scissors</t>
+  </si>
+  <si>
+    <t>good evening</t>
+  </si>
+  <si>
+    <t>how are you doing dude</t>
+  </si>
+  <si>
+    <t>what do you go by</t>
+  </si>
+  <si>
+    <t>can you tell me the name associated with this account</t>
+  </si>
+  <si>
+    <t>what version of windows am I using dude</t>
+  </si>
+  <si>
+    <t>im really sorry</t>
+  </si>
+  <si>
+    <t>am okay</t>
+  </si>
+  <si>
+    <t>alrighty your hobbies are</t>
+  </si>
+  <si>
+    <t>open up youtube</t>
+  </si>
+  <si>
+    <t>open up chat gpt</t>
+  </si>
+  <si>
+    <t>enable text to speech</t>
+  </si>
+  <si>
+    <t>mimic my speech</t>
+  </si>
+  <si>
+    <t>show me the conversion of hours into weeks</t>
+  </si>
+  <si>
+    <t>help me figure out the compound interest on my account</t>
+  </si>
+  <si>
+    <t>schedule a reminder for</t>
+  </si>
+  <si>
+    <t>please search wikipedia for a topic</t>
+  </si>
+  <si>
+    <t>choose a number at random</t>
+  </si>
+  <si>
+    <t>help me with lottery numbers</t>
+  </si>
+  <si>
+    <t>give me the outcome of a dice roll</t>
+  </si>
+  <si>
+    <t>can you make an image for me</t>
+  </si>
+  <si>
+    <t>can you analyze this for me</t>
+  </si>
+  <si>
+    <t>got any good jokes</t>
+  </si>
+  <si>
+    <t>im ready for a game of rock paper scissors</t>
+  </si>
+  <si>
+    <t>how are you today</t>
+  </si>
+  <si>
+    <t>what are you called</t>
+  </si>
+  <si>
+    <t>could you remind me what I told you my name is</t>
+  </si>
+  <si>
+    <t>can you tell me which windows os version I have</t>
+  </si>
+  <si>
+    <t>I feel bad im sorry</t>
+  </si>
+  <si>
+    <t>I am doing well</t>
+  </si>
+  <si>
+    <t>what do you do for fun</t>
+  </si>
+  <si>
+    <t>I want to watch youtube</t>
+  </si>
+  <si>
+    <t>activate text to speech</t>
+  </si>
+  <si>
+    <t>say the same thing im saying</t>
+  </si>
+  <si>
+    <t>translate hours into weeks</t>
+  </si>
+  <si>
+    <t>keep me on track with a reminder for</t>
+  </si>
+  <si>
+    <t>tell me what wikipedia says about a topic</t>
+  </si>
+  <si>
+    <t>generate a set of lottery numbers</t>
+  </si>
+  <si>
+    <t>roll a die</t>
+  </si>
+  <si>
+    <t>create a graphic</t>
+  </si>
+  <si>
+    <t>I need some analysis can you help</t>
+  </si>
+  <si>
+    <t>make me laugh please</t>
+  </si>
+  <si>
+    <t>lets settle this with rock paper scissors</t>
+  </si>
+  <si>
+    <t>hey whats up dude</t>
+  </si>
+  <si>
+    <t>how are you feeling</t>
+  </si>
+  <si>
+    <t>whats your title</t>
+  </si>
+  <si>
+    <t>do you remember the name I gave you</t>
+  </si>
+  <si>
+    <t>whats the windows os version on this computer</t>
+  </si>
+  <si>
+    <t>I want to apologize</t>
+  </si>
+  <si>
+    <t>im doing well thanks for asking</t>
+  </si>
+  <si>
+    <t>im feeling down</t>
+  </si>
+  <si>
+    <t>do you have any interests</t>
+  </si>
+  <si>
+    <t>can you open youtube for me</t>
+  </si>
+  <si>
+    <t>turn on speech synthesis</t>
+  </si>
+  <si>
+    <t>echo back what im saying</t>
+  </si>
+  <si>
+    <t>I am feeling lucky lets get some lotto numbers</t>
+  </si>
+  <si>
+    <t>I want to roll the dice</t>
+  </si>
+  <si>
+    <t>generate an illustration</t>
+  </si>
+  <si>
+    <t>analyzing this would be helpful</t>
+  </si>
+  <si>
+    <t>thanks for your help dude</t>
+  </si>
+  <si>
+    <t>entertain me with a joke please</t>
+  </si>
+  <si>
+    <t>whats the weather like today</t>
+  </si>
+  <si>
+    <t>choose your weapon rock paper or scissors</t>
+  </si>
+  <si>
+    <t>yo what is up</t>
+  </si>
+  <si>
+    <t>hows everything going</t>
+  </si>
+  <si>
+    <t>what should I call you by</t>
+  </si>
+  <si>
+    <t>im drawing a blank whats my name</t>
+  </si>
+  <si>
+    <t>im curious about my windows os version can you check</t>
+  </si>
+  <si>
+    <t>I owe you an apology</t>
+  </si>
+  <si>
+    <t>I am doing good thanks</t>
+  </si>
+  <si>
+    <t>im not doing so well</t>
+  </si>
+  <si>
+    <t>what are your hobbies bro</t>
+  </si>
+  <si>
+    <t>id like to go on youtube</t>
+  </si>
+  <si>
+    <t>start text to speech</t>
+  </si>
+  <si>
+    <t>id like you to say what I say</t>
+  </si>
+  <si>
+    <t>roll a standard dice</t>
+  </si>
+  <si>
+    <t>make me an image</t>
+  </si>
+  <si>
+    <t>merge pdf files for me</t>
+  </si>
+  <si>
+    <t>id like your analysis on this</t>
+  </si>
+  <si>
+    <t>thanks a lot dude</t>
+  </si>
+  <si>
+    <t>I need a chuckle tell me a joke</t>
+  </si>
+  <si>
+    <t>can you give me the weather forecast</t>
+  </si>
+  <si>
+    <t>I want to challenge you to a game of RPS</t>
+  </si>
+  <si>
+    <t>yo whats up</t>
+  </si>
+  <si>
+    <t>how are things</t>
+  </si>
+  <si>
+    <t>do you have a name</t>
+  </si>
+  <si>
+    <t>can you look up my name for me</t>
+  </si>
+  <si>
+    <t>which edition of windows is installed on this device</t>
+  </si>
+  <si>
+    <t>im deeply sorry</t>
+  </si>
+  <si>
+    <t>I am good dude</t>
+  </si>
+  <si>
+    <t>im feeling sad</t>
+  </si>
+  <si>
+    <t>are there any activities that you enjoy</t>
+  </si>
+  <si>
+    <t>access the youtube platform</t>
+  </si>
+  <si>
+    <t>engage text to speech mode</t>
+  </si>
+  <si>
+    <t>I want you to repeat after me</t>
+  </si>
+  <si>
+    <t>design an image for me</t>
+  </si>
+  <si>
+    <t>combine multiple pdfs</t>
+  </si>
+  <si>
+    <t>launch the application</t>
+  </si>
+  <si>
+    <t>I want an app to be closed</t>
+  </si>
+  <si>
+    <t>please analyze</t>
+  </si>
+  <si>
+    <t>I appreciate it thanks</t>
+  </si>
+  <si>
+    <t>exit the program</t>
+  </si>
+  <si>
+    <t>share a joke with me</t>
+  </si>
+  <si>
+    <t>tell me about todays weather</t>
+  </si>
+  <si>
+    <t>lets play some RPS</t>
+  </si>
+  <si>
+    <t>hi dude</t>
+  </si>
+  <si>
+    <t>hows your day been</t>
+  </si>
+  <si>
+    <t>whats your moniker</t>
+  </si>
+  <si>
+    <t>what did I enter as my name when I signed up</t>
+  </si>
+  <si>
+    <t>whats the operating system version on my pc</t>
+  </si>
+  <si>
+    <t>please forgive me</t>
+  </si>
+  <si>
+    <t>I am super well</t>
+  </si>
+  <si>
+    <t>im feeling low</t>
+  </si>
+  <si>
+    <t>any hobbies you have that youre passionate about</t>
+  </si>
+  <si>
+    <t>direct me to youtube please</t>
+  </si>
+  <si>
+    <t>enable speech output</t>
+  </si>
+  <si>
+    <t>cope me please</t>
+  </si>
+  <si>
+    <t>I want to generate a picture</t>
+  </si>
+  <si>
+    <t>I need to merge pdf documents</t>
+  </si>
+  <si>
+    <t>run the app</t>
+  </si>
+  <si>
+    <t>can you help me close an app please</t>
+  </si>
+  <si>
+    <t>analytical assistance required</t>
+  </si>
+  <si>
+    <t>thanks for the assistance</t>
+  </si>
+  <si>
+    <t>quit the application</t>
+  </si>
+  <si>
+    <t>do you know any funny jokes</t>
+  </si>
+  <si>
+    <t>I need to know the weather conditions</t>
+  </si>
+  <si>
+    <t>hey want to play rock paper scissors with me</t>
+  </si>
+  <si>
+    <t>are you doing okay</t>
+  </si>
+  <si>
+    <t>could you share your name with me</t>
+  </si>
+  <si>
+    <t>can you provide information about the windows OS version</t>
+  </si>
+  <si>
+    <t>forgive me please</t>
+  </si>
+  <si>
+    <t>today is a great day for me</t>
+  </si>
+  <si>
+    <t>im not feeling great</t>
+  </si>
+  <si>
+    <t>do you like to do anything in your freetime</t>
+  </si>
+  <si>
+    <t>take me to the youtube site</t>
+  </si>
+  <si>
+    <t>initiate text to voice</t>
+  </si>
+  <si>
+    <t>mimic me please</t>
+  </si>
+  <si>
+    <t>create a visual</t>
+  </si>
+  <si>
+    <t>can you join pdf files together</t>
+  </si>
+  <si>
+    <t>initiate the program</t>
+  </si>
+  <si>
+    <t>I need to close sommething can you close an app</t>
+  </si>
+  <si>
+    <t>can you provide some analysis</t>
+  </si>
+  <si>
+    <t>thanks for your support</t>
+  </si>
+  <si>
+    <t>hit me with a joke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">whats the weather forecast for </t>
+  </si>
+  <si>
+    <t>how are you holding up</t>
+  </si>
+  <si>
+    <t>im feeling abit blue</t>
+  </si>
+  <si>
+    <t>activate voice synthesis</t>
+  </si>
+  <si>
+    <t>please repeat after me</t>
+  </si>
+  <si>
+    <t>merge several pdfs into one</t>
+  </si>
+  <si>
+    <t>open this software</t>
+  </si>
+  <si>
+    <t xml:space="preserve">im curious about your analysis </t>
+  </si>
+  <si>
+    <t>thank you very much</t>
+  </si>
+  <si>
+    <t>end the session</t>
+  </si>
+  <si>
+    <t>im in the mood for a joke tell me one</t>
+  </si>
+  <si>
+    <t>is it going to rain today</t>
+  </si>
+  <si>
+    <t>hows life treating you</t>
+  </si>
+  <si>
+    <t>im feeling upset</t>
+  </si>
+  <si>
+    <t>switch on text to audio</t>
+  </si>
+  <si>
+    <t>combine pdf files into a single doc</t>
+  </si>
+  <si>
+    <t>run the apps</t>
+  </si>
+  <si>
+    <t>close the apps</t>
+  </si>
+  <si>
+    <t>analysis needed</t>
+  </si>
+  <si>
+    <t>im grateful thanks</t>
+  </si>
+  <si>
+    <t>terminate the session</t>
+  </si>
+  <si>
+    <t>give me an update on the forecast for today</t>
+  </si>
+  <si>
+    <t>turn on the voice reader</t>
+  </si>
+  <si>
+    <t>join my pdfs together</t>
+  </si>
+  <si>
+    <t>can you open an application for me</t>
+  </si>
+  <si>
+    <t>could you analyze this text</t>
+  </si>
+  <si>
+    <t>thanks for your time</t>
+  </si>
+  <si>
+    <t>stop</t>
+  </si>
+  <si>
+    <t>tell me if its going to be sunny</t>
+  </si>
+  <si>
+    <t>merge multiple pdf files into one for me please</t>
+  </si>
+  <si>
+    <t>can you start an app please</t>
+  </si>
+  <si>
+    <t>much appreciated thanks</t>
+  </si>
+  <si>
+    <t>shut down please</t>
+  </si>
+  <si>
+    <t>whats the temperature outside</t>
+  </si>
+  <si>
+    <t>I need to launch something can you help</t>
+  </si>
+  <si>
+    <t>thanks for everything</t>
+  </si>
+  <si>
+    <t>please shut down</t>
+  </si>
+  <si>
+    <t>im curious about the weather can you tell me</t>
+  </si>
+  <si>
+    <t>can you assist me in opening an application</t>
+  </si>
+  <si>
+    <t>wrap it up</t>
+  </si>
+  <si>
+    <t>could you initiate an app for me</t>
+  </si>
+  <si>
+    <t>finished</t>
+  </si>
+  <si>
+    <t>id like to open an application could you assist</t>
+  </si>
+  <si>
+    <t>say goodbye</t>
+  </si>
+  <si>
+    <t>can you help me launch an app</t>
+  </si>
+  <si>
+    <t>I need to start something could you open an app</t>
+  </si>
+  <si>
+    <t>could you assist me in launching an application</t>
+  </si>
+  <si>
+    <t>can you help me with an app please</t>
+  </si>
+  <si>
+    <t>I want an app to be opened</t>
+  </si>
+  <si>
+    <t>today is going quite well for me</t>
+  </si>
+  <si>
+    <t>please go ahead and repeat after what I will say</t>
   </si>
 </sst>
 </file>
@@ -1793,6 +2716,57 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AB8989F1-9511-4396-A6C2-1CF7792687C0}" name="Table1" displayName="Table1" ref="A1:AP100" totalsRowShown="0">
+  <autoFilter ref="A1:AP100" xr:uid="{AB8989F1-9511-4396-A6C2-1CF7792687C0}"/>
+  <tableColumns count="42">
+    <tableColumn id="1" xr3:uid="{8ABE6F0E-82B0-450D-8004-A121376D8BF2}" name="cls"/>
+    <tableColumn id="2" xr3:uid="{B8038201-8AAC-4F16-AA91-706A317B2594}" name="help"/>
+    <tableColumn id="3" xr3:uid="{6FBC3E0F-9AEB-429E-A141-7AE54BABEA09}" name="time"/>
+    <tableColumn id="4" xr3:uid="{F12942A7-4A5C-4055-8AAF-E33179566E47}" name="open_app"/>
+    <tableColumn id="5" xr3:uid="{83EC9054-472B-4261-94B6-75524491F386}" name="close_app"/>
+    <tableColumn id="6" xr3:uid="{CB79F2ED-1BF5-4635-820D-981BD2B44ED8}" name="analyze"/>
+    <tableColumn id="7" xr3:uid="{D50AD5E2-6854-46BF-AD4C-F0EEF89A4DD7}" name="math"/>
+    <tableColumn id="8" xr3:uid="{19F62C66-AB1B-45BC-9369-0F5E2EF1D629}" name="thanks"/>
+    <tableColumn id="9" xr3:uid="{BE10C221-9EB7-4C27-B164-D46517FF0BBB}" name="quit"/>
+    <tableColumn id="10" xr3:uid="{50FCC357-ED8D-4C84-9C26-41793C243FC3}" name="tell_joke"/>
+    <tableColumn id="11" xr3:uid="{CFEFE155-C4A1-4E47-AA10-CCCC18FB3FEE}" name="weather"/>
+    <tableColumn id="12" xr3:uid="{69BFEEC8-39FF-44AA-B9B9-F1E289E5E51F}" name="rock_paper_scissors"/>
+    <tableColumn id="13" xr3:uid="{7507E41C-7136-4BF4-932A-8CBE286EC4AF}" name="greetings"/>
+    <tableColumn id="14" xr3:uid="{8911E4D8-BD00-4C4C-A178-7EDD0E81BD75}" name="how_are_you"/>
+    <tableColumn id="15" xr3:uid="{D90201F3-BE86-46D0-818A-505D25E34198}" name="what_is_your_name"/>
+    <tableColumn id="16" xr3:uid="{3E764299-C284-429A-8702-DE186DDE4413}" name="my_name"/>
+    <tableColumn id="17" xr3:uid="{FA58D2E7-9C14-4B63-AAA7-75FBF746A618}" name="windows"/>
+    <tableColumn id="18" xr3:uid="{E46028B3-33B5-4721-AADA-340A053F0B97}" name="sorry"/>
+    <tableColumn id="19" xr3:uid="{E449B236-0C82-49F9-8BFC-60A8116C7853}" name="feeling_good"/>
+    <tableColumn id="20" xr3:uid="{690E0B3A-2EAC-4D10-93D8-080A87ACC18C}" name="feeling_bad"/>
+    <tableColumn id="21" xr3:uid="{63570C01-6837-4DD3-BD56-B2BA74FE2628}" name="discuss_hobbies"/>
+    <tableColumn id="22" xr3:uid="{4B262020-998C-4179-A793-245A1033F6DA}" name="xac_hellven"/>
+    <tableColumn id="23" xr3:uid="{4DB73827-A9A7-438A-8784-02CFA7287C89}" name="youtube"/>
+    <tableColumn id="24" xr3:uid="{F7C40981-5E05-458B-8EC4-E042757B1B20}" name="GPT"/>
+    <tableColumn id="25" xr3:uid="{3369E653-EA34-4BC1-8F8D-46D632164D11}" name="enable_tts"/>
+    <tableColumn id="26" xr3:uid="{1873A256-D445-46FD-8B03-4D660D1A032A}" name="disable_tts"/>
+    <tableColumn id="27" xr3:uid="{A8BC9EEC-3FB6-4885-AF00-D501813B44A4}" name="angry"/>
+    <tableColumn id="28" xr3:uid="{797103E1-857C-4D8E-971A-41144FA62A6B}" name="copy"/>
+    <tableColumn id="29" xr3:uid="{1D40CC0A-3D8F-46E4-92A8-A4E864EA2496}" name="time_conversion"/>
+    <tableColumn id="30" xr3:uid="{7DBB3E9C-E841-4617-B546-D220641AA3EC}" name="calculate_compound_interest"/>
+    <tableColumn id="31" xr3:uid="{13024436-4408-4C0B-8FE2-9C9870AF0D27}" name="remind"/>
+    <tableColumn id="32" xr3:uid="{1EACAA06-07A3-4881-9278-0EAEE996AB63}" name="wiki"/>
+    <tableColumn id="33" xr3:uid="{E13E6777-CD8B-48BB-8370-B6E80960AF15}" name="random_number"/>
+    <tableColumn id="34" xr3:uid="{E808A63F-716A-4E22-B08C-76C71FEFEEA2}" name="lottery"/>
+    <tableColumn id="35" xr3:uid="{08E960B6-CC16-466D-BF71-B103D3B3E862}" name="dice"/>
+    <tableColumn id="36" xr3:uid="{084EB521-1F3E-486C-9F7B-9F5AFB38AA78}" name="image_generator"/>
+    <tableColumn id="37" xr3:uid="{B780E3F4-1426-4E44-BE92-4C5D74053D29}" name="merge_pdfs"/>
+    <tableColumn id="38" xr3:uid="{F8461DA5-1091-44B8-BE8E-CB5546165424}" name="pass_check"/>
+    <tableColumn id="39" xr3:uid="{2BD59183-5A1B-470A-ABE1-05EF995D8F03}" name="png_to_pdf"/>
+    <tableColumn id="40" xr3:uid="{A85EC536-BB4A-4269-AF73-AEB1FA395EA0}" name="say_something"/>
+    <tableColumn id="41" xr3:uid="{237029E5-09D5-4C59-90A2-647108EE029C}" name="start_pomo"/>
+    <tableColumn id="42" xr3:uid="{4C50BBE5-FA03-4AC8-9D62-56B67FD0ADC7}" name="stop_pomo"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2112,10 +3086,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69FDA376-956F-4742-8649-35ECB5332B72}">
-  <dimension ref="A1:AP91"/>
+  <dimension ref="A1:AP92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB12" sqref="AB12"/>
+      <selection activeCell="AB23" sqref="AB23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2366,6 +3340,9 @@
       <c r="AM2" t="s">
         <v>351</v>
       </c>
+      <c r="AN2" t="s">
+        <v>509</v>
+      </c>
       <c r="AO2" t="s">
         <v>353</v>
       </c>
@@ -2595,6 +3572,9 @@
       <c r="AF4" t="s">
         <v>324</v>
       </c>
+      <c r="AG4" t="s">
+        <v>574</v>
+      </c>
       <c r="AH4" t="s">
         <v>332</v>
       </c>
@@ -2708,11 +3688,17 @@
       <c r="AC5" t="s">
         <v>314</v>
       </c>
+      <c r="AD5" t="s">
+        <v>575</v>
+      </c>
       <c r="AE5" t="s">
         <v>321</v>
       </c>
       <c r="AF5" t="s">
         <v>325</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>576</v>
       </c>
       <c r="AH5" t="s">
         <v>333</v>
@@ -2782,6 +3768,12 @@
       <c r="N6" t="s">
         <v>210</v>
       </c>
+      <c r="O6" t="s">
+        <v>568</v>
+      </c>
+      <c r="P6" t="s">
+        <v>577</v>
+      </c>
       <c r="Q6" t="s">
         <v>222</v>
       </c>
@@ -2818,8 +3810,23 @@
       <c r="AB6" t="s">
         <v>308</v>
       </c>
+      <c r="AC6" t="s">
+        <v>578</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>579</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>580</v>
+      </c>
       <c r="AF6" t="s">
         <v>326</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>581</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>582</v>
       </c>
       <c r="AI6" t="s">
         <v>338</v>
@@ -2877,9 +3884,18 @@
       <c r="K7" t="s">
         <v>187</v>
       </c>
+      <c r="M7" t="s">
+        <v>583</v>
+      </c>
       <c r="N7" t="s">
         <v>11</v>
       </c>
+      <c r="O7" t="s">
+        <v>569</v>
+      </c>
+      <c r="P7" t="s">
+        <v>584</v>
+      </c>
       <c r="Q7" t="s">
         <v>558</v>
       </c>
@@ -2916,8 +3932,23 @@
       <c r="AB7" t="s">
         <v>309</v>
       </c>
+      <c r="AC7" t="s">
+        <v>585</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>586</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>587</v>
+      </c>
       <c r="AF7" t="s">
         <v>327</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>588</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>589</v>
       </c>
       <c r="AI7" t="s">
         <v>339</v>
@@ -2975,15 +4006,30 @@
       <c r="K8" t="s">
         <v>188</v>
       </c>
+      <c r="L8" t="s">
+        <v>590</v>
+      </c>
+      <c r="M8" t="s">
+        <v>591</v>
+      </c>
       <c r="N8" t="s">
         <v>478</v>
       </c>
+      <c r="O8" t="s">
+        <v>570</v>
+      </c>
+      <c r="P8" t="s">
+        <v>592</v>
+      </c>
       <c r="Q8" t="s">
         <v>559</v>
       </c>
       <c r="R8" t="s">
         <v>228</v>
       </c>
+      <c r="S8" t="s">
+        <v>593</v>
+      </c>
       <c r="T8" t="s">
         <v>239</v>
       </c>
@@ -3010,6 +4056,27 @@
       </c>
       <c r="AB8" t="s">
         <v>310</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>594</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>595</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>596</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>597</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>598</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>599</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>600</v>
       </c>
       <c r="AJ8" t="s">
         <v>532</v>
@@ -3064,15 +4131,30 @@
       <c r="K9" t="s">
         <v>189</v>
       </c>
+      <c r="L9" t="s">
+        <v>601</v>
+      </c>
+      <c r="M9" t="s">
+        <v>602</v>
+      </c>
       <c r="N9" t="s">
         <v>210</v>
       </c>
+      <c r="O9" t="s">
+        <v>571</v>
+      </c>
+      <c r="P9" t="s">
+        <v>603</v>
+      </c>
       <c r="Q9" t="s">
         <v>560</v>
       </c>
       <c r="R9" t="s">
         <v>229</v>
       </c>
+      <c r="S9" t="s">
+        <v>604</v>
+      </c>
       <c r="T9" t="s">
         <v>551</v>
       </c>
@@ -3099,6 +4181,27 @@
       </c>
       <c r="AB9" t="s">
         <v>565</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>605</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>606</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>607</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>608</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>609</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>610</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>611</v>
       </c>
       <c r="AJ9" t="s">
         <v>533</v>
@@ -3153,12 +4256,30 @@
       <c r="K10" t="s">
         <v>190</v>
       </c>
+      <c r="L10" t="s">
+        <v>612</v>
+      </c>
+      <c r="M10" t="s">
+        <v>613</v>
+      </c>
       <c r="N10" t="s">
         <v>479</v>
       </c>
+      <c r="O10" t="s">
+        <v>572</v>
+      </c>
+      <c r="P10" t="s">
+        <v>614</v>
+      </c>
       <c r="Q10" t="s">
         <v>561</v>
       </c>
+      <c r="R10" t="s">
+        <v>615</v>
+      </c>
+      <c r="S10" t="s">
+        <v>616</v>
+      </c>
       <c r="T10" t="s">
         <v>552</v>
       </c>
@@ -3168,6 +4289,12 @@
       <c r="V10" t="s">
         <v>474</v>
       </c>
+      <c r="W10" t="s">
+        <v>617</v>
+      </c>
+      <c r="X10" t="s">
+        <v>618</v>
+      </c>
       <c r="Y10" t="s">
         <v>269</v>
       </c>
@@ -3179,6 +4306,27 @@
       </c>
       <c r="AB10" t="s">
         <v>566</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>619</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>620</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>621</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>622</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>623</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>624</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>625</v>
       </c>
       <c r="AJ10" t="s">
         <v>534</v>
@@ -3233,18 +4381,45 @@
       <c r="K11" t="s">
         <v>191</v>
       </c>
+      <c r="L11" t="s">
+        <v>626</v>
+      </c>
+      <c r="M11" t="s">
+        <v>627</v>
+      </c>
       <c r="N11" t="s">
         <v>480</v>
       </c>
+      <c r="O11" t="s">
+        <v>628</v>
+      </c>
+      <c r="P11" t="s">
+        <v>629</v>
+      </c>
       <c r="Q11" t="s">
         <v>562</v>
       </c>
+      <c r="R11" t="s">
+        <v>630</v>
+      </c>
+      <c r="S11" t="s">
+        <v>631</v>
+      </c>
       <c r="T11" t="s">
         <v>553</v>
       </c>
+      <c r="U11" t="s">
+        <v>632</v>
+      </c>
       <c r="V11" t="s">
         <v>475</v>
       </c>
+      <c r="W11" t="s">
+        <v>633</v>
+      </c>
+      <c r="X11" t="s">
+        <v>634</v>
+      </c>
       <c r="Y11" t="s">
         <v>466</v>
       </c>
@@ -3256,6 +4431,30 @@
       </c>
       <c r="AB11" t="s">
         <v>567</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>635</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>636</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>637</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>638</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>639</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>640</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>641</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>642</v>
       </c>
       <c r="AK11" t="s">
         <v>523</v>
@@ -3304,18 +4503,45 @@
       <c r="K12" t="s">
         <v>192</v>
       </c>
+      <c r="L12" t="s">
+        <v>643</v>
+      </c>
+      <c r="M12" t="s">
+        <v>644</v>
+      </c>
       <c r="N12" t="s">
         <v>481</v>
       </c>
+      <c r="O12" t="s">
+        <v>645</v>
+      </c>
+      <c r="P12" t="s">
+        <v>646</v>
+      </c>
       <c r="Q12" t="s">
         <v>563</v>
       </c>
+      <c r="R12" t="s">
+        <v>647</v>
+      </c>
+      <c r="S12" t="s">
+        <v>648</v>
+      </c>
       <c r="T12" t="s">
         <v>554</v>
       </c>
+      <c r="U12" t="s">
+        <v>649</v>
+      </c>
       <c r="V12" t="s">
         <v>476</v>
       </c>
+      <c r="W12" t="s">
+        <v>650</v>
+      </c>
+      <c r="X12" t="s">
+        <v>651</v>
+      </c>
       <c r="Y12" t="s">
         <v>467</v>
       </c>
@@ -3324,6 +4550,33 @@
       </c>
       <c r="AA12" t="s">
         <v>298</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>652</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>653</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>654</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>655</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>656</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>657</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>658</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>659</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>660</v>
       </c>
       <c r="AK12" t="s">
         <v>524</v>
@@ -3366,18 +4619,48 @@
       <c r="I13" t="s">
         <v>165</v>
       </c>
+      <c r="J13" t="s">
+        <v>661</v>
+      </c>
       <c r="K13" t="s">
         <v>193</v>
       </c>
+      <c r="L13" t="s">
+        <v>662</v>
+      </c>
+      <c r="M13" t="s">
+        <v>663</v>
+      </c>
       <c r="N13" t="s">
         <v>482</v>
       </c>
+      <c r="O13" t="s">
+        <v>664</v>
+      </c>
+      <c r="P13" t="s">
+        <v>665</v>
+      </c>
+      <c r="R13" t="s">
+        <v>666</v>
+      </c>
+      <c r="S13" t="s">
+        <v>667</v>
+      </c>
       <c r="T13" t="s">
         <v>555</v>
       </c>
+      <c r="U13" t="s">
+        <v>668</v>
+      </c>
       <c r="V13" t="s">
         <v>477</v>
       </c>
+      <c r="W13" t="s">
+        <v>669</v>
+      </c>
+      <c r="X13" t="s">
+        <v>670</v>
+      </c>
       <c r="Y13" t="s">
         <v>468</v>
       </c>
@@ -3386,6 +4669,33 @@
       </c>
       <c r="AA13" t="s">
         <v>299</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>671</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>672</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>673</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>674</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>675</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>676</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>677</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>678</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>679</v>
       </c>
       <c r="AK13" t="s">
         <v>525</v>
@@ -3428,17 +4738,83 @@
       <c r="I14" t="s">
         <v>166</v>
       </c>
+      <c r="J14" t="s">
+        <v>680</v>
+      </c>
       <c r="K14" t="s">
         <v>194</v>
       </c>
+      <c r="L14" t="s">
+        <v>681</v>
+      </c>
+      <c r="M14" t="s">
+        <v>682</v>
+      </c>
+      <c r="N14" t="s">
+        <v>683</v>
+      </c>
+      <c r="O14" t="s">
+        <v>684</v>
+      </c>
+      <c r="P14" t="s">
+        <v>685</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>686</v>
+      </c>
+      <c r="R14" t="s">
+        <v>687</v>
+      </c>
+      <c r="S14" t="s">
+        <v>688</v>
+      </c>
       <c r="T14" t="s">
         <v>556</v>
       </c>
+      <c r="U14" t="s">
+        <v>689</v>
+      </c>
+      <c r="W14" t="s">
+        <v>690</v>
+      </c>
+      <c r="X14" t="s">
+        <v>691</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>692</v>
+      </c>
       <c r="Z14" t="s">
         <v>281</v>
       </c>
       <c r="AA14" t="s">
         <v>300</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>693</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>694</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>695</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>696</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>697</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>698</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>699</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>700</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>701</v>
       </c>
       <c r="AK14" t="s">
         <v>526</v>
@@ -3469,6 +4845,9 @@
       <c r="D15" t="s">
         <v>459</v>
       </c>
+      <c r="F15" t="s">
+        <v>702</v>
+      </c>
       <c r="G15" t="s">
         <v>133</v>
       </c>
@@ -3478,17 +4857,71 @@
       <c r="I15" t="s">
         <v>167</v>
       </c>
+      <c r="J15" t="s">
+        <v>703</v>
+      </c>
       <c r="K15" t="s">
         <v>195</v>
       </c>
+      <c r="L15" t="s">
+        <v>704</v>
+      </c>
+      <c r="N15" t="s">
+        <v>705</v>
+      </c>
+      <c r="O15" t="s">
+        <v>706</v>
+      </c>
+      <c r="P15" t="s">
+        <v>707</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>708</v>
+      </c>
+      <c r="R15" t="s">
+        <v>709</v>
+      </c>
+      <c r="S15" t="s">
+        <v>710</v>
+      </c>
       <c r="T15" t="s">
         <v>557</v>
       </c>
+      <c r="U15" t="s">
+        <v>711</v>
+      </c>
+      <c r="W15" t="s">
+        <v>712</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>713</v>
+      </c>
       <c r="Z15" t="s">
         <v>282</v>
       </c>
       <c r="AA15" t="s">
         <v>301</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>714</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>715</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>716</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>717</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>718</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>719</v>
+      </c>
+      <c r="AJ15" t="s">
+        <v>720</v>
       </c>
       <c r="AK15" t="s">
         <v>527</v>
@@ -3510,6 +4943,9 @@
       <c r="D16" t="s">
         <v>460</v>
       </c>
+      <c r="F16" t="s">
+        <v>721</v>
+      </c>
       <c r="G16" t="s">
         <v>134</v>
       </c>
@@ -3519,20 +4955,71 @@
       <c r="I16" t="s">
         <v>168</v>
       </c>
+      <c r="J16" t="s">
+        <v>722</v>
+      </c>
       <c r="K16" t="s">
         <v>196</v>
       </c>
+      <c r="L16" t="s">
+        <v>723</v>
+      </c>
+      <c r="M16" t="s">
+        <v>724</v>
+      </c>
+      <c r="N16" t="s">
+        <v>725</v>
+      </c>
+      <c r="O16" t="s">
+        <v>726</v>
+      </c>
+      <c r="P16" t="s">
+        <v>727</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>728</v>
+      </c>
+      <c r="R16" t="s">
+        <v>729</v>
+      </c>
+      <c r="S16" t="s">
+        <v>730</v>
+      </c>
+      <c r="T16" t="s">
+        <v>731</v>
+      </c>
+      <c r="U16" t="s">
+        <v>732</v>
+      </c>
+      <c r="W16" t="s">
+        <v>733</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>734</v>
+      </c>
       <c r="Z16" t="s">
         <v>283</v>
       </c>
       <c r="AA16" t="s">
         <v>302</v>
       </c>
+      <c r="AB16" t="s">
+        <v>735</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>736</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>737</v>
+      </c>
+      <c r="AJ16" t="s">
+        <v>738</v>
+      </c>
       <c r="AK16" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>84</v>
       </c>
@@ -3545,20 +5032,80 @@
       <c r="D17" t="s">
         <v>461</v>
       </c>
+      <c r="F17" t="s">
+        <v>739</v>
+      </c>
       <c r="G17" t="s">
         <v>135</v>
       </c>
+      <c r="H17" t="s">
+        <v>740</v>
+      </c>
       <c r="I17" t="s">
         <v>169</v>
       </c>
+      <c r="J17" t="s">
+        <v>741</v>
+      </c>
+      <c r="K17" t="s">
+        <v>742</v>
+      </c>
+      <c r="L17" t="s">
+        <v>743</v>
+      </c>
+      <c r="M17" t="s">
+        <v>744</v>
+      </c>
+      <c r="N17" t="s">
+        <v>745</v>
+      </c>
+      <c r="O17" t="s">
+        <v>746</v>
+      </c>
+      <c r="P17" t="s">
+        <v>747</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>748</v>
+      </c>
+      <c r="R17" t="s">
+        <v>749</v>
+      </c>
+      <c r="S17" t="s">
+        <v>750</v>
+      </c>
+      <c r="T17" t="s">
+        <v>751</v>
+      </c>
+      <c r="U17" t="s">
+        <v>752</v>
+      </c>
+      <c r="W17" t="s">
+        <v>753</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>754</v>
+      </c>
       <c r="Z17" t="s">
         <v>284</v>
       </c>
       <c r="AA17" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB17" t="s">
+        <v>755</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>756</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>757</v>
+      </c>
+      <c r="AK17" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>85</v>
       </c>
@@ -3571,17 +5118,74 @@
       <c r="D18" t="s">
         <v>462</v>
       </c>
+      <c r="F18" t="s">
+        <v>759</v>
+      </c>
       <c r="G18" t="s">
         <v>136</v>
       </c>
+      <c r="H18" t="s">
+        <v>760</v>
+      </c>
       <c r="I18" t="s">
         <v>170</v>
       </c>
+      <c r="J18" t="s">
+        <v>761</v>
+      </c>
+      <c r="K18" t="s">
+        <v>762</v>
+      </c>
+      <c r="L18" t="s">
+        <v>763</v>
+      </c>
+      <c r="M18" t="s">
+        <v>764</v>
+      </c>
+      <c r="N18" t="s">
+        <v>765</v>
+      </c>
+      <c r="O18" t="s">
+        <v>766</v>
+      </c>
+      <c r="P18" t="s">
+        <v>767</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>768</v>
+      </c>
+      <c r="R18" t="s">
+        <v>769</v>
+      </c>
+      <c r="S18" t="s">
+        <v>770</v>
+      </c>
+      <c r="T18" t="s">
+        <v>771</v>
+      </c>
+      <c r="U18" t="s">
+        <v>772</v>
+      </c>
+      <c r="W18" t="s">
+        <v>773</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>774</v>
+      </c>
       <c r="Z18" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB18" t="s">
+        <v>775</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>776</v>
+      </c>
+      <c r="AK18" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>86</v>
       </c>
@@ -3591,14 +5195,80 @@
       <c r="C19" t="s">
         <v>94</v>
       </c>
+      <c r="D19" t="s">
+        <v>778</v>
+      </c>
+      <c r="E19" t="s">
+        <v>779</v>
+      </c>
+      <c r="F19" t="s">
+        <v>780</v>
+      </c>
       <c r="G19" t="s">
         <v>137</v>
       </c>
+      <c r="H19" t="s">
+        <v>781</v>
+      </c>
+      <c r="I19" t="s">
+        <v>782</v>
+      </c>
+      <c r="J19" t="s">
+        <v>783</v>
+      </c>
+      <c r="K19" t="s">
+        <v>784</v>
+      </c>
+      <c r="L19" t="s">
+        <v>785</v>
+      </c>
+      <c r="M19" t="s">
+        <v>786</v>
+      </c>
+      <c r="N19" t="s">
+        <v>787</v>
+      </c>
+      <c r="O19" t="s">
+        <v>788</v>
+      </c>
+      <c r="P19" t="s">
+        <v>789</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>790</v>
+      </c>
+      <c r="R19" t="s">
+        <v>791</v>
+      </c>
+      <c r="S19" t="s">
+        <v>792</v>
+      </c>
+      <c r="T19" t="s">
+        <v>793</v>
+      </c>
+      <c r="U19" t="s">
+        <v>794</v>
+      </c>
+      <c r="W19" t="s">
+        <v>795</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>796</v>
+      </c>
       <c r="Z19" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB19" t="s">
+        <v>797</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>798</v>
+      </c>
+      <c r="AK19" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>363</v>
       </c>
@@ -3608,14 +5278,74 @@
       <c r="C20" t="s">
         <v>95</v>
       </c>
+      <c r="D20" t="s">
+        <v>800</v>
+      </c>
+      <c r="E20" t="s">
+        <v>801</v>
+      </c>
+      <c r="F20" t="s">
+        <v>802</v>
+      </c>
       <c r="G20" t="s">
         <v>138</v>
       </c>
+      <c r="H20" t="s">
+        <v>803</v>
+      </c>
+      <c r="I20" t="s">
+        <v>804</v>
+      </c>
+      <c r="J20" t="s">
+        <v>805</v>
+      </c>
+      <c r="K20" t="s">
+        <v>806</v>
+      </c>
+      <c r="L20" t="s">
+        <v>807</v>
+      </c>
+      <c r="N20" t="s">
+        <v>808</v>
+      </c>
+      <c r="O20" t="s">
+        <v>809</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>810</v>
+      </c>
+      <c r="R20" t="s">
+        <v>811</v>
+      </c>
+      <c r="S20" t="s">
+        <v>812</v>
+      </c>
+      <c r="T20" t="s">
+        <v>813</v>
+      </c>
+      <c r="U20" t="s">
+        <v>814</v>
+      </c>
+      <c r="W20" t="s">
+        <v>815</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>816</v>
+      </c>
       <c r="Z20" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB20" t="s">
+        <v>817</v>
+      </c>
+      <c r="AJ20" t="s">
+        <v>818</v>
+      </c>
+      <c r="AK20" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>364</v>
       </c>
@@ -3625,14 +5355,53 @@
       <c r="C21" t="s">
         <v>443</v>
       </c>
+      <c r="D21" t="s">
+        <v>820</v>
+      </c>
+      <c r="E21" t="s">
+        <v>821</v>
+      </c>
+      <c r="F21" t="s">
+        <v>822</v>
+      </c>
       <c r="G21" t="s">
         <v>139</v>
       </c>
+      <c r="H21" t="s">
+        <v>823</v>
+      </c>
+      <c r="I21" t="s">
+        <v>159</v>
+      </c>
+      <c r="J21" t="s">
+        <v>824</v>
+      </c>
+      <c r="K21" t="s">
+        <v>825</v>
+      </c>
+      <c r="N21" t="s">
+        <v>826</v>
+      </c>
+      <c r="S21" t="s">
+        <v>874</v>
+      </c>
+      <c r="T21" t="s">
+        <v>827</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>828</v>
+      </c>
       <c r="Z21" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB21" t="s">
+        <v>829</v>
+      </c>
+      <c r="AK21" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>365</v>
       </c>
@@ -3642,11 +5411,47 @@
       <c r="C22" t="s">
         <v>444</v>
       </c>
+      <c r="D22" t="s">
+        <v>831</v>
+      </c>
+      <c r="E22" t="s">
+        <v>801</v>
+      </c>
+      <c r="F22" t="s">
+        <v>832</v>
+      </c>
       <c r="G22" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>833</v>
+      </c>
+      <c r="I22" t="s">
+        <v>834</v>
+      </c>
+      <c r="J22" t="s">
+        <v>835</v>
+      </c>
+      <c r="K22" t="s">
+        <v>836</v>
+      </c>
+      <c r="N22" t="s">
+        <v>837</v>
+      </c>
+      <c r="T22" t="s">
+        <v>838</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>839</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>875</v>
+      </c>
+      <c r="AK22" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>366</v>
       </c>
@@ -3656,11 +5461,35 @@
       <c r="C23" t="s">
         <v>445</v>
       </c>
+      <c r="D23" t="s">
+        <v>841</v>
+      </c>
+      <c r="E23" t="s">
+        <v>842</v>
+      </c>
+      <c r="F23" t="s">
+        <v>843</v>
+      </c>
       <c r="G23" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>844</v>
+      </c>
+      <c r="I23" t="s">
+        <v>845</v>
+      </c>
+      <c r="K23" t="s">
+        <v>846</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>847</v>
+      </c>
+      <c r="AK23" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>367</v>
       </c>
@@ -3670,11 +5499,29 @@
       <c r="C24" t="s">
         <v>446</v>
       </c>
+      <c r="D24" t="s">
+        <v>849</v>
+      </c>
+      <c r="F24" t="s">
+        <v>850</v>
+      </c>
       <c r="G24" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>851</v>
+      </c>
+      <c r="I24" t="s">
+        <v>852</v>
+      </c>
+      <c r="K24" t="s">
+        <v>853</v>
+      </c>
+      <c r="AK24" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>368</v>
       </c>
@@ -3684,8 +5531,20 @@
       <c r="C25" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>855</v>
+      </c>
+      <c r="H25" t="s">
+        <v>856</v>
+      </c>
+      <c r="I25" t="s">
+        <v>857</v>
+      </c>
+      <c r="K25" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>369</v>
       </c>
@@ -3695,8 +5554,20 @@
       <c r="C26" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>859</v>
+      </c>
+      <c r="H26" t="s">
+        <v>860</v>
+      </c>
+      <c r="I26" t="s">
+        <v>861</v>
+      </c>
+      <c r="K26" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>370</v>
       </c>
@@ -3706,8 +5577,14 @@
       <c r="C27" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>863</v>
+      </c>
+      <c r="I27" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>371</v>
       </c>
@@ -3717,8 +5594,14 @@
       <c r="C28" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>865</v>
+      </c>
+      <c r="I28" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>372</v>
       </c>
@@ -3728,8 +5611,14 @@
       <c r="C29" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>867</v>
+      </c>
+      <c r="I29" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>373</v>
       </c>
@@ -3739,105 +5628,120 @@
       <c r="C30" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>374</v>
       </c>
       <c r="B31" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>375</v>
       </c>
       <c r="B32" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>376</v>
       </c>
       <c r="B33" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>377</v>
       </c>
       <c r="B34" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>391</v>
       </c>
@@ -4057,8 +5961,16 @@
         <v>384</v>
       </c>
     </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>573</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>